<commit_message>
New data and changes to R script after Day2 larval sampling
</commit_message>
<xml_diff>
--- a/Trial2_docs/20160306_Experimental_Work.xlsx
+++ b/Trial2_docs/20160306_Experimental_Work.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19480" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19480" windowHeight="14900" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="66">
   <si>
     <t>Sunday</t>
   </si>
@@ -105,12 +105,6 @@
     <t>cells.per.ml</t>
   </si>
   <si>
-    <t>Average.Alive</t>
-  </si>
-  <si>
-    <t>Average.Dead</t>
-  </si>
-  <si>
     <t>Live1</t>
   </si>
   <si>
@@ -135,30 +129,9 @@
     <t>Dead4</t>
   </si>
   <si>
-    <t>live.larvae.per.ml</t>
-  </si>
-  <si>
-    <t>ml.for.sample</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Percent.Alive</t>
-  </si>
-  <si>
-    <t>Percent.Dead</t>
-  </si>
-  <si>
     <t>Volume.Counted.ml</t>
   </si>
   <si>
-    <t>Total.Volume.ml</t>
-  </si>
-  <si>
-    <t>Total.Live.Larvae</t>
-  </si>
-  <si>
     <t>Bottle #</t>
   </si>
   <si>
@@ -204,12 +177,6 @@
     <t>Header2</t>
   </si>
   <si>
-    <t>na</t>
-  </si>
-  <si>
-    <t>Initial Batch</t>
-  </si>
-  <si>
     <t>Live5</t>
   </si>
   <si>
@@ -232,16 +199,36 @@
   </si>
   <si>
     <t>Water Chem and Maint</t>
+  </si>
+  <si>
+    <t>Requested TA</t>
+  </si>
+  <si>
+    <t>Requested pH</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Vol.Tripour</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Ambient</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -322,7 +309,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="122">
+  <cellStyleXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -445,14 +432,104 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -472,8 +549,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="122">
+  <cellStyles count="214">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -535,6 +613,52 @@
     <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -595,6 +719,52 @@
     <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -926,7 +1096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView showRuler="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -936,300 +1106,300 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="18">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7">
         <v>1</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <v>2</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <v>3</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="7">
         <v>4</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15" customHeight="1">
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" s="10"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="8"/>
     </row>
     <row r="6" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="B6" s="9">
+      <c r="B6" s="7">
         <v>6</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="7">
         <v>7</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="7">
         <v>8</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>9</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="7">
         <v>10</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="7">
         <v>11</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="7">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="15" customHeight="1">
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="15" customHeight="1">
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>68</v>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="B9" s="9">
+      <c r="B9" s="7">
         <v>13</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="7">
         <v>14</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="7">
         <v>15</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="7">
         <v>16</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <v>17</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <v>18</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="7">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="15" customHeight="1">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="10" t="s">
+      <c r="C10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="15" customHeight="1">
-      <c r="B11" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>66</v>
+      <c r="B11" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="B12" s="9">
+      <c r="B12" s="7">
         <v>20</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="7">
         <v>21</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="7">
         <v>22</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="7">
         <v>23</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="7">
         <v>24</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="7">
         <v>25</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="7">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="15" customHeight="1">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="15" customHeight="1">
-      <c r="B14" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>69</v>
+      <c r="B14" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="2:8" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="B15" s="9">
+      <c r="B15" s="7">
         <v>27</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="7">
         <v>28</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="7">
         <v>29</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="7">
         <v>30</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="7">
         <v>31</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
     </row>
     <row r="16" spans="2:8" ht="15" customHeight="1">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="2:4">
-      <c r="B17" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>68</v>
+      <c r="B17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1245,19 +1415,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C2" sqref="C2:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="8" max="8" width="15.1640625" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1265,211 +1440,640 @@
         <v>19</v>
       </c>
       <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>20160308</v>
       </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2">
         <v>75</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>84</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>97</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>87</v>
       </c>
-      <c r="G2">
-        <f>AVERAGE(C2:F2)</f>
+      <c r="H2">
+        <f>AVERAGE(D2:G2)</f>
         <v>85.75</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="I2" s="2">
-        <f>G2/H2</f>
+      <c r="J2" s="2">
+        <f>H2/I2</f>
         <v>95277.777777777781</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>20160308</v>
       </c>
-      <c r="B3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3">
         <v>106</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>114</v>
       </c>
-      <c r="E3" t="s">
-        <v>60</v>
-      </c>
       <c r="F3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G7" si="0">AVERAGE(C3:F3)</f>
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H19" si="0">AVERAGE(D3:G3)</f>
         <v>110</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="I3" s="2">
-        <f t="shared" ref="I3:I7" si="1">G3/H3</f>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:J7" si="1">H3/I3</f>
         <v>122222.22222222222</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>20160308</v>
       </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4">
         <v>113</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>115</v>
       </c>
-      <c r="E4" t="s">
-        <v>60</v>
-      </c>
       <c r="F4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4">
+        <v>61</v>
+      </c>
+      <c r="G4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4">
         <f t="shared" si="0"/>
         <v>114</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <f t="shared" si="1"/>
         <v>126666.66666666667</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>20160308</v>
       </c>
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5">
         <v>112</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>93</v>
       </c>
-      <c r="E5" t="s">
-        <v>60</v>
-      </c>
       <c r="F5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5">
+        <v>61</v>
+      </c>
+      <c r="G5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="0"/>
         <v>102.5</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <f t="shared" si="1"/>
         <v>113888.88888888889</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>20160308</v>
       </c>
-      <c r="B6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6">
         <v>103</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>115</v>
       </c>
-      <c r="E6" t="s">
-        <v>60</v>
-      </c>
       <c r="F6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6">
+        <v>61</v>
+      </c>
+      <c r="G6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="0"/>
         <v>109</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <f t="shared" si="1"/>
         <v>121111.11111111111</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>20160308</v>
       </c>
-      <c r="B7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7">
         <v>115</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>84</v>
       </c>
-      <c r="E7" t="s">
-        <v>60</v>
-      </c>
       <c r="F7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7">
+        <v>61</v>
+      </c>
+      <c r="G7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="0"/>
         <v>99.5</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <f t="shared" si="1"/>
         <v>110555.55555555556</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>20160309</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8">
+        <v>143</v>
+      </c>
+      <c r="E8">
+        <v>159</v>
+      </c>
+      <c r="F8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>151</v>
+      </c>
+      <c r="I8">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" ref="J8:J19" si="2">H8/I8</f>
+        <v>167777.77777777778</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9">
+        <v>20160309</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9">
+        <v>158</v>
+      </c>
+      <c r="E9">
+        <v>140</v>
+      </c>
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>149</v>
+      </c>
+      <c r="I9">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="2"/>
+        <v>165555.55555555556</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10">
+        <v>20160309</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10">
+        <v>145</v>
+      </c>
+      <c r="E10">
+        <v>177</v>
+      </c>
+      <c r="F10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>161</v>
+      </c>
+      <c r="I10">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="2"/>
+        <v>178888.88888888891</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11">
+        <v>20160309</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11">
+        <v>126</v>
+      </c>
+      <c r="E11">
+        <v>119</v>
+      </c>
+      <c r="F11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>122.5</v>
+      </c>
+      <c r="I11">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="2"/>
+        <v>136111.11111111112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12">
+        <v>20160309</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12">
+        <v>126</v>
+      </c>
+      <c r="E12">
+        <v>115</v>
+      </c>
+      <c r="F12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>120.5</v>
+      </c>
+      <c r="I12">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="2"/>
+        <v>133888.88888888891</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13">
+        <v>20160309</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13">
+        <v>119</v>
+      </c>
+      <c r="E13">
+        <v>121</v>
+      </c>
+      <c r="F13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="I13">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="2"/>
+        <v>133333.33333333334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14">
+        <v>20160310</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14">
+        <v>113</v>
+      </c>
+      <c r="E14">
+        <v>150</v>
+      </c>
+      <c r="F14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>131.5</v>
+      </c>
+      <c r="I14">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="2"/>
+        <v>146111.11111111112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15">
+        <v>20160310</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15">
+        <v>117</v>
+      </c>
+      <c r="E15">
+        <v>123</v>
+      </c>
+      <c r="F15" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="I15">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="2"/>
+        <v>133333.33333333334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16">
+        <v>20160310</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16">
+        <v>128</v>
+      </c>
+      <c r="E16">
+        <v>134</v>
+      </c>
+      <c r="F16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>131</v>
+      </c>
+      <c r="I16">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="2"/>
+        <v>145555.55555555556</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>20160310</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17">
+        <v>136</v>
+      </c>
+      <c r="E17">
+        <v>116</v>
+      </c>
+      <c r="F17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="I17">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="2"/>
+        <v>140000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>20160310</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18">
+        <v>133</v>
+      </c>
+      <c r="E18">
+        <v>127</v>
+      </c>
+      <c r="F18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="I18">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="2"/>
+        <v>144444.44444444444</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>20160310</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19">
+        <v>153</v>
+      </c>
+      <c r="E19">
+        <v>139</v>
+      </c>
+      <c r="F19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="I19">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="2"/>
+        <v>162222.22222222222</v>
       </c>
     </row>
   </sheetData>
@@ -1485,37 +2089,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="6.5" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="6.5" customWidth="1"/>
+    <col min="14" max="14" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5" customWidth="1"/>
+    <col min="17" max="17" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1">
+    <row r="1" spans="1:17" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1523,206 +2120,611 @@
         <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
-      <c r="A2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2">
+        <v>20160308</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
       </c>
       <c r="D2">
-        <v>110</v>
-      </c>
-      <c r="E2">
-        <v>101</v>
+        <v>113</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
       </c>
       <c r="F2">
-        <v>111</v>
-      </c>
-      <c r="G2">
-        <v>102</v>
+        <v>119</v>
+      </c>
+      <c r="G2" t="s">
+        <v>61</v>
       </c>
       <c r="H2">
-        <v>112</v>
-      </c>
-      <c r="I2">
-        <v>103</v>
+        <v>124</v>
+      </c>
+      <c r="I2" t="s">
+        <v>61</v>
       </c>
       <c r="J2">
-        <v>113</v>
-      </c>
-      <c r="K2">
-        <v>110</v>
+        <v>126</v>
+      </c>
+      <c r="K2" t="s">
+        <v>61</v>
       </c>
       <c r="L2">
-        <v>110</v>
-      </c>
-      <c r="M2">
-        <f>AVERAGE(C2,E2,G2,I2,K2)</f>
-        <v>103.2</v>
+        <v>126</v>
+      </c>
+      <c r="M2" t="s">
+        <v>61</v>
       </c>
       <c r="N2">
-        <f>AVERAGE(D2,F2,H2,J2,L2)</f>
-        <v>111.2</v>
-      </c>
-      <c r="O2" s="3">
-        <f>(M2/SUM(M2:N2))*100</f>
-        <v>48.134328358208954</v>
-      </c>
-      <c r="P2" s="3">
-        <f>100-O2</f>
-        <v>51.865671641791046</v>
-      </c>
-      <c r="Q2">
-        <v>0.1</v>
-      </c>
-      <c r="R2">
-        <v>800</v>
-      </c>
-      <c r="S2">
-        <f>M2/Q2</f>
-        <v>1032</v>
-      </c>
-      <c r="T2" s="5">
-        <f>S2*R2</f>
-        <v>825600</v>
-      </c>
-      <c r="U2" s="4">
-        <f>10000/S2</f>
-        <v>9.6899224806201545</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
+        <v>0.2</v>
+      </c>
+      <c r="O2">
+        <v>1892.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>20160308</v>
       </c>
-      <c r="B3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3">
         <v>113</v>
       </c>
-      <c r="D3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3">
         <v>119</v>
       </c>
-      <c r="F3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3">
+      <c r="G3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3">
         <v>124</v>
       </c>
-      <c r="H3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3">
+      <c r="I3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3">
         <v>126</v>
       </c>
-      <c r="J3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K3">
+      <c r="K3" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3">
         <v>126</v>
       </c>
-      <c r="L3" t="s">
-        <v>60</v>
-      </c>
-      <c r="M3">
-        <f>AVERAGE(C3,E3,G3,I3,K3)</f>
-        <v>121.6</v>
-      </c>
-      <c r="N3" t="e">
-        <f>AVERAGE(D3,F3,H3,J3,L3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O3" s="3" t="e">
-        <f>(M3/SUM(M3:N3))*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P3" s="3" t="e">
-        <f>100-O3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q3">
+      <c r="M3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3">
         <v>0.2</v>
       </c>
-      <c r="R3">
-        <f>11.3562*1000</f>
-        <v>11356.199999999999</v>
-      </c>
-      <c r="S3">
-        <f>M3/Q3</f>
-        <v>607.99999999999989</v>
-      </c>
-      <c r="T3" s="5">
-        <f>S3*R3</f>
-        <v>6904569.5999999978</v>
-      </c>
-      <c r="U3" s="4">
-        <f>10000/S3</f>
-        <v>16.447368421052634</v>
+      <c r="O3">
+        <v>1892.7</v>
+      </c>
+      <c r="Q3" s="11">
+        <f>1150761.6*6</f>
+        <v>6904569.6000000006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4">
+        <v>20160308</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4">
+        <v>113</v>
+      </c>
+      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4">
+        <v>119</v>
+      </c>
+      <c r="G4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4">
+        <v>124</v>
+      </c>
+      <c r="I4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4">
+        <v>126</v>
+      </c>
+      <c r="K4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L4">
+        <v>126</v>
+      </c>
+      <c r="M4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4">
+        <v>0.2</v>
+      </c>
+      <c r="O4">
+        <v>1892.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5">
+        <v>20160308</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5">
+        <v>113</v>
+      </c>
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5">
+        <v>119</v>
+      </c>
+      <c r="G5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5">
+        <v>124</v>
+      </c>
+      <c r="I5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5">
+        <v>126</v>
+      </c>
+      <c r="K5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5">
+        <v>126</v>
+      </c>
+      <c r="M5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N5">
+        <v>0.2</v>
+      </c>
+      <c r="O5">
+        <v>1892.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6">
+        <v>20160308</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6">
+        <v>113</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6">
+        <v>119</v>
+      </c>
+      <c r="G6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6">
+        <v>124</v>
+      </c>
+      <c r="I6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6">
+        <v>126</v>
+      </c>
+      <c r="K6" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6">
+        <v>126</v>
+      </c>
+      <c r="M6" t="s">
+        <v>61</v>
+      </c>
+      <c r="N6">
+        <v>0.2</v>
+      </c>
+      <c r="O6">
+        <v>1892.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7">
+        <v>20160308</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7">
+        <v>113</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7">
+        <v>119</v>
+      </c>
+      <c r="G7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7">
+        <v>124</v>
+      </c>
+      <c r="I7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7">
+        <v>126</v>
+      </c>
+      <c r="K7" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7">
+        <v>126</v>
+      </c>
+      <c r="M7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7">
+        <v>0.2</v>
+      </c>
+      <c r="O7">
+        <v>1892.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8">
+        <v>20160310</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8">
+        <v>208</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>221</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>209</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" t="s">
+        <v>61</v>
+      </c>
+      <c r="M8" t="s">
+        <v>61</v>
+      </c>
+      <c r="N8">
+        <v>0.1</v>
+      </c>
+      <c r="O8">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9">
+        <v>20160310</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9">
+        <v>228</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>184</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>188</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" t="s">
+        <v>61</v>
+      </c>
+      <c r="M9" t="s">
+        <v>61</v>
+      </c>
+      <c r="N9">
+        <v>0.1</v>
+      </c>
+      <c r="O9">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10">
+        <v>20160310</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10">
+        <v>198</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>190</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>231</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" t="s">
+        <v>61</v>
+      </c>
+      <c r="M10" t="s">
+        <v>61</v>
+      </c>
+      <c r="N10">
+        <v>0.1</v>
+      </c>
+      <c r="O10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11">
+        <v>20160310</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11">
+        <v>207</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>222</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>199</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11" t="s">
+        <v>61</v>
+      </c>
+      <c r="K11" t="s">
+        <v>61</v>
+      </c>
+      <c r="L11" t="s">
+        <v>61</v>
+      </c>
+      <c r="M11" t="s">
+        <v>61</v>
+      </c>
+      <c r="N11">
+        <v>0.1</v>
+      </c>
+      <c r="O11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12">
+        <v>20160310</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12">
+        <v>148</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>199</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>180</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" t="s">
+        <v>61</v>
+      </c>
+      <c r="L12" t="s">
+        <v>61</v>
+      </c>
+      <c r="M12" t="s">
+        <v>61</v>
+      </c>
+      <c r="N12">
+        <v>0.1</v>
+      </c>
+      <c r="O12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13">
+        <v>20160310</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13">
+        <v>192</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>182</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>197</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>61</v>
+      </c>
+      <c r="K13" t="s">
+        <v>61</v>
+      </c>
+      <c r="L13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M13" t="s">
+        <v>61</v>
+      </c>
+      <c r="N13">
+        <v>0.1</v>
+      </c>
+      <c r="O13">
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -1738,10 +2740,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H181"/>
+  <dimension ref="A1:J181"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1754,46 +2756,54 @@
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>38</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>20160308</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="4">
         <v>0.4458333333333333</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E2">
         <v>14.05</v>
@@ -1804,22 +2814,25 @@
       <c r="G2">
         <v>27.5</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="4">
         <v>0.46875</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2">
+        <v>20160309</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>20160308</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="4">
         <v>0.4458333333333333</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E3">
         <v>14.05</v>
@@ -1830,22 +2843,22 @@
       <c r="G3">
         <v>27.5</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="4">
         <v>0.46875</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>20160308</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <v>0.44930555555555557</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E4">
         <v>14.06</v>
@@ -1856,22 +2869,25 @@
       <c r="G4">
         <v>27.5</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="4">
         <v>0.46875</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <v>20160309</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>20160308</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>0.44930555555555557</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E5">
         <v>14.06</v>
@@ -1882,22 +2898,22 @@
       <c r="G5">
         <v>27.5</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="4">
         <v>0.46875</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>20160308</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <v>0.45208333333333334</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E6">
         <v>14.14</v>
@@ -1908,22 +2924,25 @@
       <c r="G6">
         <v>27.5</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="4">
         <v>0.46875</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6">
+        <v>20160309</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>20160308</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="4">
         <v>0.45208333333333334</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E7">
         <v>14.14</v>
@@ -1934,24 +2953,24 @@
       <c r="G7">
         <v>27.5</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="4">
         <v>0.46875</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>20160308</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <v>0.43541666666666662</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="4">
+        <v>46</v>
+      </c>
+      <c r="E8" s="3">
         <v>14.11</v>
       </c>
       <c r="F8">
@@ -1960,24 +2979,27 @@
       <c r="G8">
         <v>27.5</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="4">
         <v>0.46875</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8">
+        <v>20160309</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>20160308</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="4">
         <v>0.43541666666666662</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="4">
+        <v>46</v>
+      </c>
+      <c r="E9" s="3">
         <v>14.11</v>
       </c>
       <c r="F9">
@@ -1986,22 +3008,22 @@
       <c r="G9">
         <v>27.5</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="4">
         <v>0.46875</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>20160308</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <v>0.43888888888888888</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E10">
         <v>14.1</v>
@@ -2012,22 +3034,25 @@
       <c r="G10">
         <v>27.5</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="4">
         <v>0.46875</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10">
+        <v>20160309</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>20160308</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="4">
         <v>0.43888888888888888</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E11">
         <v>14.1</v>
@@ -2038,22 +3063,22 @@
       <c r="G11">
         <v>27.5</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="4">
         <v>0.46875</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <v>20160308</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <v>0.44236111111111115</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E12">
         <v>14.08</v>
@@ -2064,22 +3089,25 @@
       <c r="G12">
         <v>27.5</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="4">
         <v>0.46875</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12">
+        <v>20160309</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <v>20160308</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="4">
         <v>0.44236111111111115</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E13">
         <v>14.08</v>
@@ -2090,22 +3118,22 @@
       <c r="G13">
         <v>27.5</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="4">
         <v>0.46875</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
         <v>20160308</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="4">
         <v>0.42708333333333331</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E14">
         <v>13.73</v>
@@ -2116,22 +3144,28 @@
       <c r="G14">
         <v>27.4</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="4">
         <v>0.46875</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14">
+        <v>20160309</v>
+      </c>
+      <c r="J14">
+        <v>20160309</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <v>20160308</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="4">
         <v>0.42708333333333331</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E15">
         <v>13.73</v>
@@ -2142,22 +3176,22 @@
       <c r="G15">
         <v>27.4</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="4">
         <v>0.46875</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <v>20160308</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="4">
         <v>0.43263888888888885</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E16">
         <v>13.68</v>
@@ -2168,22 +3202,28 @@
       <c r="G16">
         <v>27.6</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="4">
         <v>0.46875</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16">
+        <v>20160309</v>
+      </c>
+      <c r="J16">
+        <v>20160309</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
         <v>20160308</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="4">
         <v>0.43263888888888885</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E17">
         <v>13.68</v>
@@ -2194,161 +3234,527 @@
       <c r="G17">
         <v>27.6</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="4">
         <v>0.46875</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="B18">
+        <v>20160309</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18">
+        <v>13.31</v>
+      </c>
+      <c r="F18">
+        <v>-28.3</v>
+      </c>
+      <c r="G18">
+        <v>27.5</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="I18">
+        <v>20160309</v>
+      </c>
+      <c r="J18">
+        <v>20160309</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="B19">
+        <v>20160309</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19">
+        <v>13.31</v>
+      </c>
+      <c r="F19">
+        <v>-28.3</v>
+      </c>
+      <c r="G19">
+        <v>27.5</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0.54513888888888895</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="B20">
+        <v>20160309</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.48888888888888887</v>
+      </c>
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20">
+        <v>13.3</v>
+      </c>
+      <c r="F20">
+        <v>-55.5</v>
+      </c>
+      <c r="G20">
+        <v>27.5</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="I20">
+        <v>20160309</v>
+      </c>
+      <c r="J20">
+        <v>20160309</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="B21">
+        <v>20160309</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.48888888888888887</v>
+      </c>
+      <c r="D21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21">
+        <v>13.3</v>
+      </c>
+      <c r="F21">
+        <v>-55.5</v>
+      </c>
+      <c r="G21">
+        <v>27.5</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0.54513888888888895</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="B22">
+        <v>20160309</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22">
+        <v>13.93</v>
+      </c>
+      <c r="F22">
+        <v>-29</v>
+      </c>
+      <c r="G22">
+        <v>27.4</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="I22">
+        <v>20160309</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="B23">
+        <v>20160309</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23">
+        <v>13.93</v>
+      </c>
+      <c r="F23">
+        <v>-29</v>
+      </c>
+      <c r="G23">
+        <v>27.4</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0.54513888888888895</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="B24">
+        <v>20160309</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.51944444444444449</v>
+      </c>
+      <c r="D24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24">
+        <v>13.92</v>
+      </c>
+      <c r="F24">
+        <v>-55</v>
+      </c>
+      <c r="G24">
+        <v>27.4</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="I24">
+        <v>20160309</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="B25">
+        <v>20160309</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.51944444444444449</v>
+      </c>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25">
+        <v>13.92</v>
+      </c>
+      <c r="F25">
+        <v>-55</v>
+      </c>
+      <c r="G25">
+        <v>27.4</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0.54513888888888895</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="B26">
+        <v>20160309</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="D26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26">
+        <v>13.93</v>
+      </c>
+      <c r="F26">
+        <v>-55</v>
+      </c>
+      <c r="G26">
+        <v>27.4</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="I26">
+        <v>20160309</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="B27">
+        <v>20160309</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="D27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27">
+        <v>13.93</v>
+      </c>
+      <c r="F27">
+        <v>-55</v>
+      </c>
+      <c r="G27">
+        <v>27.4</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0.54513888888888895</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="B28">
+        <v>20160309</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.49652777777777773</v>
+      </c>
+      <c r="D28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28">
+        <v>13.91</v>
+      </c>
+      <c r="F28">
+        <v>-28.2</v>
+      </c>
+      <c r="G28">
+        <v>27.4</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="I28">
+        <v>20160309</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="B29">
+        <v>20160309</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.49652777777777773</v>
+      </c>
+      <c r="D29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29">
+        <v>13.91</v>
+      </c>
+      <c r="F29">
+        <v>-28.2</v>
+      </c>
+      <c r="G29">
+        <v>27.4</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0.54513888888888895</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="B30">
+        <v>20160309</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="D30" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30">
+        <v>13.93</v>
+      </c>
+      <c r="F30">
+        <v>-28.6</v>
+      </c>
+      <c r="G30">
+        <v>27.5</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="I30">
+        <v>20160309</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="B31">
+        <v>20160309</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="D31" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31">
+        <v>13.93</v>
+      </c>
+      <c r="F31">
+        <v>-28.6</v>
+      </c>
+      <c r="G31">
+        <v>27.5</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0.54513888888888895</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32">
+        <v>20160309</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.50902777777777775</v>
+      </c>
+      <c r="D32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32">
+        <v>13.94</v>
+      </c>
+      <c r="F32">
+        <v>-55</v>
+      </c>
+      <c r="G32">
+        <v>27.4</v>
+      </c>
+      <c r="H32" s="4">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="I32">
+        <v>20160309</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="B33">
+        <v>20160309</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.50902777777777775</v>
+      </c>
+      <c r="D33" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33">
+        <v>13.94</v>
+      </c>
+      <c r="F33">
+        <v>-55</v>
+      </c>
+      <c r="G33">
+        <v>27.4</v>
+      </c>
+      <c r="H33" s="4">
+        <v>0.54513888888888895</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:8">
       <c r="A35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:8">
       <c r="A36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:8">
       <c r="A37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:8">
       <c r="A38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:8">
       <c r="A39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:8">
       <c r="A40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:8">
       <c r="A41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:8">
       <c r="A42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:8">
       <c r="A43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:8">
       <c r="A44">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:8">
       <c r="A45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:8">
       <c r="A46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:8">
       <c r="A47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:8">
       <c r="A48">
         <v>47</v>
       </c>

</xml_diff>